<commit_message>
Removed an empty line.
</commit_message>
<xml_diff>
--- a/recipeData/CombineRecipes.xlsx
+++ b/recipeData/CombineRecipes.xlsx
@@ -1397,9 +1397,6 @@
     <t>vegetable oil; onions; screw pine leaves (daun pandan); 1 kg lean beef; coconut cream (santan pekat); water; tamarind pulp; desiccated coconut (kerisik); sugar; Salt</t>
   </si>
   <si>
-    <t>Oven; ;Brass moulds</t>
-  </si>
-  <si>
     <t>ghee; plain flour</t>
   </si>
   <si>
@@ -2400,6 +2397,9 @@
   </si>
   <si>
     <t>Clams in Chinese rice wine ginger and chili</t>
+  </si>
+  <si>
+    <t>Oven;Brass moulds</t>
   </si>
 </sst>
 </file>
@@ -2826,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2836,7 +2836,7 @@
     <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="8" max="9" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.140625" style="17" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -2912,7 +2912,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>15</v>
@@ -2930,12 +2930,12 @@
         <v>324</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="17" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>17</v>
@@ -2976,14 +2976,14 @@
         <v>329</v>
       </c>
       <c r="L3" s="17" t="s">
+        <v>504</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>505</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>506</v>
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="17" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>19</v>
@@ -3024,12 +3024,12 @@
         <v>331</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>22</v>
@@ -3070,14 +3070,14 @@
         <v>333</v>
       </c>
       <c r="L5" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="M5" s="17" t="s">
         <v>509</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>510</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>25</v>
@@ -3118,14 +3118,14 @@
         <v>336</v>
       </c>
       <c r="L6" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>512</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>513</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="17" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>27</v>
@@ -3163,17 +3163,17 @@
         <v>335</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L7" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="M7" s="17" t="s">
         <v>515</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>516</v>
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="17" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>30</v>
@@ -3211,12 +3211,12 @@
         <v>34</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>35</v>
@@ -3257,16 +3257,16 @@
         <v>338</v>
       </c>
       <c r="L9" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="N9" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="O9" s="17" t="s">
         <v>521</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>522</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>39</v>
@@ -3292,7 +3292,7 @@
         <v>341</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>90</v>
@@ -3307,14 +3307,14 @@
         <v>340</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M10" s="15" t="s">
         <v>41</v>
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>42</v>
@@ -3337,10 +3337,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>81</v>
@@ -3355,14 +3355,14 @@
         <v>343</v>
       </c>
       <c r="L11" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>525</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>526</v>
       </c>
       <c r="N11" s="15"/>
       <c r="O11" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>46</v>
@@ -3403,12 +3403,12 @@
         <v>345</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="17" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>48</v>
@@ -3449,14 +3449,14 @@
         <v>348</v>
       </c>
       <c r="L13" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="M13" s="17" t="s">
         <v>529</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>530</v>
       </c>
       <c r="N13" s="15"/>
       <c r="O13" s="17" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>50</v>
@@ -3497,16 +3497,16 @@
         <v>351</v>
       </c>
       <c r="L14" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="M14" s="17" t="s">
         <v>531</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>532</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>319</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>52</v>
@@ -3547,14 +3547,14 @@
         <v>353</v>
       </c>
       <c r="L15" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="M15" s="17" t="s">
         <v>533</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>534</v>
       </c>
       <c r="N15" s="15"/>
       <c r="O15" s="17" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>54</v>
@@ -3595,12 +3595,12 @@
         <v>355</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="17" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>56</v>
@@ -3641,14 +3641,14 @@
         <v>357</v>
       </c>
       <c r="L17" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="M17" s="17" t="s">
         <v>536</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>537</v>
       </c>
       <c r="N17" s="15"/>
       <c r="O17" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>58</v>
@@ -3689,12 +3689,12 @@
         <v>359</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>60</v>
@@ -3735,12 +3735,12 @@
         <v>362</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="15"/>
       <c r="O19" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>62</v>
@@ -3781,12 +3781,12 @@
         <v>364</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="15"/>
       <c r="O20" s="17" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>64</v>
@@ -3827,12 +3827,12 @@
         <v>367</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M21" s="17"/>
       <c r="N21" s="15"/>
       <c r="O21" s="17" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>66</v>
@@ -3840,7 +3840,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>322</v>
@@ -3858,7 +3858,7 @@
         <v>371</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>81</v>
@@ -3873,14 +3873,14 @@
         <v>370</v>
       </c>
       <c r="L22" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="M22" s="17" t="s">
         <v>542</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>543</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="17" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>68</v>
@@ -3921,11 +3921,11 @@
         <v>373</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="M23" s="24"/>
       <c r="O23" s="24" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="P23" s="25" t="s">
         <v>71</v>
@@ -3966,13 +3966,13 @@
         <v>376</v>
       </c>
       <c r="L24" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="M24" s="24" t="s">
         <v>545</v>
       </c>
-      <c r="M24" s="24" t="s">
+      <c r="O24" s="24" t="s">
         <v>546</v>
-      </c>
-      <c r="O24" s="24" t="s">
-        <v>547</v>
       </c>
       <c r="P24" s="25" t="s">
         <v>75</v>
@@ -3995,7 +3995,7 @@
         <v>60</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>77</v>
@@ -4013,13 +4013,13 @@
         <v>381</v>
       </c>
       <c r="L25" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="M25" s="17" t="s">
         <v>548</v>
       </c>
-      <c r="M25" s="17" t="s">
+      <c r="O25" s="17" t="s">
         <v>549</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>550</v>
       </c>
       <c r="P25" s="15" t="s">
         <v>78</v>
@@ -4060,10 +4060,10 @@
         <v>384</v>
       </c>
       <c r="L26" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="O26" s="17" t="s">
         <v>551</v>
-      </c>
-      <c r="O26" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>84</v>
@@ -4104,10 +4104,10 @@
         <v>385</v>
       </c>
       <c r="L27" s="17" t="s">
+        <v>552</v>
+      </c>
+      <c r="O27" s="17" t="s">
         <v>553</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>554</v>
       </c>
       <c r="P27" s="15" t="s">
         <v>87</v>
@@ -4148,10 +4148,10 @@
         <v>388</v>
       </c>
       <c r="L28" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="O28" s="17" t="s">
         <v>555</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>556</v>
       </c>
       <c r="P28" s="15" t="s">
         <v>92</v>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="29" spans="1:16" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>320</v>
@@ -4192,10 +4192,10 @@
         <v>390</v>
       </c>
       <c r="L29" s="17" t="s">
+        <v>556</v>
+      </c>
+      <c r="O29" s="17" t="s">
         <v>557</v>
-      </c>
-      <c r="O29" s="17" t="s">
-        <v>558</v>
       </c>
       <c r="P29" s="15" t="s">
         <v>94</v>
@@ -4236,13 +4236,13 @@
         <v>391</v>
       </c>
       <c r="L30" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="M30" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="M30" s="17" t="s">
-        <v>560</v>
-      </c>
       <c r="O30" s="17" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="P30" s="15" t="s">
         <v>97</v>
@@ -4283,10 +4283,10 @@
         <v>393</v>
       </c>
       <c r="L31" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="O31" s="17" t="s">
         <v>561</v>
-      </c>
-      <c r="O31" s="17" t="s">
-        <v>562</v>
       </c>
       <c r="P31" s="15" t="s">
         <v>100</v>
@@ -4327,16 +4327,16 @@
         <v>396</v>
       </c>
       <c r="L32" s="17" t="s">
+        <v>562</v>
+      </c>
+      <c r="M32" s="17" t="s">
         <v>563</v>
       </c>
-      <c r="M32" s="17" t="s">
+      <c r="N32" s="17" t="s">
         <v>564</v>
       </c>
-      <c r="N32" s="17" t="s">
+      <c r="O32" s="17" t="s">
         <v>565</v>
-      </c>
-      <c r="O32" s="17" t="s">
-        <v>566</v>
       </c>
       <c r="P32" s="15" t="s">
         <v>102</v>
@@ -4377,10 +4377,10 @@
         <v>399</v>
       </c>
       <c r="L33" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="O33" s="17" t="s">
         <v>567</v>
-      </c>
-      <c r="O33" s="17" t="s">
-        <v>568</v>
       </c>
       <c r="P33" s="15" t="s">
         <v>105</v>
@@ -4421,10 +4421,10 @@
         <v>403</v>
       </c>
       <c r="L34" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="O34" s="17" t="s">
         <v>569</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>570</v>
       </c>
       <c r="P34" s="15" t="s">
         <v>108</v>
@@ -4465,10 +4465,10 @@
         <v>404</v>
       </c>
       <c r="L35" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="O35" s="17" t="s">
         <v>571</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>572</v>
       </c>
       <c r="P35" s="15" t="s">
         <v>110</v>
@@ -4509,10 +4509,10 @@
         <v>406</v>
       </c>
       <c r="L36" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="O36" s="17" t="s">
         <v>573</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>574</v>
       </c>
       <c r="P36" s="15" t="s">
         <v>113</v>
@@ -4553,10 +4553,10 @@
         <v>407</v>
       </c>
       <c r="L37" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="O37" s="17" t="s">
         <v>575</v>
-      </c>
-      <c r="O37" s="17" t="s">
-        <v>576</v>
       </c>
       <c r="P37" s="15" t="s">
         <v>115</v>
@@ -4597,10 +4597,10 @@
         <v>408</v>
       </c>
       <c r="L38" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="O38" s="17" t="s">
         <v>577</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>578</v>
       </c>
       <c r="P38" s="15" t="s">
         <v>118</v>
@@ -4638,13 +4638,13 @@
         <v>409</v>
       </c>
       <c r="L39" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="M39" s="17" t="s">
         <v>579</v>
       </c>
-      <c r="M39" s="17" t="s">
+      <c r="O39" s="17" t="s">
         <v>580</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>581</v>
       </c>
       <c r="P39" s="15" t="s">
         <v>120</v>
@@ -4685,10 +4685,10 @@
         <v>410</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="P40" s="15" t="s">
         <v>122</v>
@@ -4729,10 +4729,10 @@
         <v>411</v>
       </c>
       <c r="L41" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="O41" s="17" t="s">
         <v>583</v>
-      </c>
-      <c r="O41" s="17" t="s">
-        <v>584</v>
       </c>
       <c r="P41" s="15" t="s">
         <v>124</v>
@@ -4755,7 +4755,7 @@
         <v>15</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G42" s="15" t="s">
         <v>74</v>
@@ -4773,10 +4773,10 @@
         <v>415</v>
       </c>
       <c r="L42" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="O42" s="17" t="s">
         <v>585</v>
-      </c>
-      <c r="O42" s="17" t="s">
-        <v>586</v>
       </c>
       <c r="P42" s="15" t="s">
         <v>128</v>
@@ -4799,7 +4799,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G43" s="15" t="s">
         <v>130</v>
@@ -4814,10 +4814,10 @@
         <v>416</v>
       </c>
       <c r="L43" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="O43" s="17" t="s">
         <v>708</v>
-      </c>
-      <c r="O43" s="17" t="s">
-        <v>709</v>
       </c>
       <c r="P43" s="15" t="s">
         <v>132</v>
@@ -4858,12 +4858,12 @@
         <v>417</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="P44" s="4" t="s">
         <v>135</v>
@@ -4904,12 +4904,12 @@
         <v>420</v>
       </c>
       <c r="L45" s="17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P45" s="4" t="s">
         <v>139</v>
@@ -4950,12 +4950,12 @@
         <v>421</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="P46" s="4" t="s">
         <v>142</v>
@@ -4996,12 +4996,12 @@
         <v>423</v>
       </c>
       <c r="L47" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
       <c r="O47" s="17" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="P47" s="4" t="s">
         <v>147</v>
@@ -5042,12 +5042,12 @@
         <v>424</v>
       </c>
       <c r="L48" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
       <c r="O48" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P48" s="4" t="s">
         <v>150</v>
@@ -5088,12 +5088,12 @@
         <v>425</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="P49" s="4" t="s">
         <v>154</v>
@@ -5134,12 +5134,12 @@
         <v>428</v>
       </c>
       <c r="L50" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P50" s="4" t="s">
         <v>158</v>
@@ -5180,12 +5180,12 @@
         <v>430</v>
       </c>
       <c r="L51" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="17" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P51" s="4" t="s">
         <v>162</v>
@@ -5226,12 +5226,12 @@
         <v>431</v>
       </c>
       <c r="L52" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
       <c r="O52" s="17" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P52" s="4" t="s">
         <v>165</v>
@@ -5272,12 +5272,12 @@
         <v>432</v>
       </c>
       <c r="L53" s="17" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
       <c r="O53" s="17" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P53" s="4" t="s">
         <v>167</v>
@@ -5318,12 +5318,12 @@
         <v>435</v>
       </c>
       <c r="L54" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
       <c r="O54" s="17" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="P54" s="4" t="s">
         <v>170</v>
@@ -5361,15 +5361,15 @@
         <v>437</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="L55" s="17" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
       <c r="O55" s="17" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="P55" s="4" t="s">
         <v>174</v>
@@ -5407,15 +5407,15 @@
         <v>16</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="L56" s="17" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
       <c r="O56" s="17" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="P56" s="4" t="s">
         <v>177</v>
@@ -5456,12 +5456,12 @@
         <v>438</v>
       </c>
       <c r="L57" s="17" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
       <c r="O57" s="17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P57" s="4" t="s">
         <v>180</v>
@@ -5502,12 +5502,12 @@
         <v>439</v>
       </c>
       <c r="L58" s="17" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="P58" s="4" t="s">
         <v>182</v>
@@ -5545,15 +5545,15 @@
         <v>443</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="L59" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
       <c r="O59" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="P59" s="4" t="s">
         <v>184</v>
@@ -5591,15 +5591,15 @@
         <v>24</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L60" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
       <c r="O60" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="P60" s="4" t="s">
         <v>186</v>
@@ -5625,7 +5625,7 @@
         <v>418</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H61" s="15" t="s">
         <v>188</v>
@@ -5637,15 +5637,15 @@
         <v>146</v>
       </c>
       <c r="K61" s="17" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="L61" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
       <c r="O61" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="P61" s="4" t="s">
         <v>189</v>
@@ -5683,15 +5683,15 @@
         <v>447</v>
       </c>
       <c r="K62" s="17" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L62" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
       <c r="O62" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="P62" s="4" t="s">
         <v>192</v>
@@ -5729,17 +5729,17 @@
         <v>194</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L63" s="20" t="s">
+        <v>614</v>
+      </c>
+      <c r="M63" s="20" t="s">
         <v>615</v>
-      </c>
-      <c r="M63" s="20" t="s">
-        <v>616</v>
       </c>
       <c r="N63" s="11"/>
       <c r="O63" s="20" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="P63" s="11" t="s">
         <v>195</v>
@@ -5777,17 +5777,17 @@
         <v>24</v>
       </c>
       <c r="K64" s="11" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L64" s="20" t="s">
+        <v>616</v>
+      </c>
+      <c r="M64" s="20" t="s">
         <v>617</v>
-      </c>
-      <c r="M64" s="20" t="s">
-        <v>618</v>
       </c>
       <c r="N64" s="11"/>
       <c r="O64" s="20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="P64" s="11" t="s">
         <v>198</v>
@@ -5825,19 +5825,19 @@
         <v>200</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L65" s="20" t="s">
+        <v>619</v>
+      </c>
+      <c r="M65" s="20" t="s">
         <v>620</v>
       </c>
-      <c r="M65" s="20" t="s">
-        <v>621</v>
-      </c>
       <c r="N65" s="11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="O65" s="20" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="P65" s="11" t="s">
         <v>201</v>
@@ -5866,7 +5866,7 @@
         <v>32</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>457</v>
+        <v>791</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>21</v>
@@ -5875,17 +5875,17 @@
         <v>146</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L66" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="M66" s="20" t="s">
         <v>622</v>
-      </c>
-      <c r="M66" s="20" t="s">
-        <v>623</v>
       </c>
       <c r="N66" s="11"/>
       <c r="O66" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="P66" s="11" t="s">
         <v>203</v>
@@ -5926,12 +5926,12 @@
         <v>444</v>
       </c>
       <c r="L67" s="20" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="20" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="P67" s="11" t="s">
         <v>205</v>
@@ -5954,7 +5954,7 @@
         <v>10</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>206</v>
@@ -5972,12 +5972,12 @@
         <v>445</v>
       </c>
       <c r="L68" s="20" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="M68" s="11"/>
       <c r="N68" s="11"/>
       <c r="O68" s="20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="P68" s="11" t="s">
         <v>207</v>
@@ -6018,12 +6018,12 @@
         <v>448</v>
       </c>
       <c r="L69" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="M69" s="11"/>
       <c r="N69" s="11"/>
       <c r="O69" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="P69" s="11" t="s">
         <v>209</v>
@@ -6052,24 +6052,24 @@
         <v>32</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>211</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K70" s="11" t="s">
         <v>451</v>
       </c>
       <c r="L70" s="20" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="M70" s="11"/>
       <c r="N70" s="11"/>
       <c r="O70" s="20" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>212</v>
@@ -6104,18 +6104,18 @@
         <v>21</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K71" s="11" t="s">
         <v>455</v>
       </c>
       <c r="L71" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="P71" s="11" t="s">
         <v>214</v>
@@ -6150,18 +6150,18 @@
         <v>21</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K72" s="11" t="s">
         <v>456</v>
       </c>
       <c r="L72" s="20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
       <c r="O72" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="P72" s="11" t="s">
         <v>216</v>
@@ -6187,7 +6187,7 @@
         <v>218</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>241</v>
@@ -6199,16 +6199,16 @@
         <v>24</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L73" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="M73" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="M73" s="17" t="s">
-        <v>633</v>
-      </c>
       <c r="O73" s="17" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="P73" s="9" t="s">
         <v>219</v>
@@ -6234,7 +6234,7 @@
         <v>218</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>141</v>
@@ -6246,13 +6246,13 @@
         <v>427</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="O74" s="8" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="P74" s="9" t="s">
         <v>221</v>
@@ -6278,7 +6278,7 @@
         <v>218</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>90</v>
@@ -6287,16 +6287,16 @@
         <v>211</v>
       </c>
       <c r="J75" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L75" s="17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="O75" s="8" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="P75" s="9" t="s">
         <v>223</v>
@@ -6322,7 +6322,7 @@
         <v>218</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>312</v>
@@ -6331,22 +6331,22 @@
         <v>44</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L76" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="M76" s="17" t="s">
         <v>636</v>
       </c>
-      <c r="M76" s="17" t="s">
+      <c r="N76" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="N76" s="8" t="s">
-        <v>638</v>
-      </c>
       <c r="O76" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="P76" s="9" t="s">
         <v>225</v>
@@ -6372,7 +6372,7 @@
         <v>218</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>227</v>
@@ -6381,19 +6381,19 @@
         <v>44</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L77" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="M77" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="M77" s="8" t="s">
-        <v>640</v>
-      </c>
       <c r="O77" s="8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="P77" s="9" t="s">
         <v>228</v>
@@ -6419,7 +6419,7 @@
         <v>218</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>227</v>
@@ -6428,19 +6428,19 @@
         <v>44</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L78" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="P78" s="9" t="s">
         <v>230</v>
@@ -6466,7 +6466,7 @@
         <v>218</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H79" s="8" t="s">
         <v>90</v>
@@ -6478,16 +6478,16 @@
         <v>200</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L79" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="M79" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="M79" s="8" t="s">
-        <v>643</v>
-      </c>
       <c r="O79" s="17" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="P79" s="9" t="s">
         <v>232</v>
@@ -6513,7 +6513,7 @@
         <v>218</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>90</v>
@@ -6525,16 +6525,16 @@
         <v>200</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L80" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="M80" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="M80" s="8" t="s">
-        <v>645</v>
-      </c>
       <c r="O80" s="8" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="P80" s="9" t="s">
         <v>234</v>
@@ -6560,7 +6560,7 @@
         <v>218</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>241</v>
@@ -6572,16 +6572,16 @@
         <v>236</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L81" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="M81" s="17" t="s">
         <v>646</v>
       </c>
-      <c r="M81" s="17" t="s">
-        <v>647</v>
-      </c>
       <c r="O81" s="10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="P81" s="9" t="s">
         <v>237</v>
@@ -6613,25 +6613,25 @@
         <v>241</v>
       </c>
       <c r="I82" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J82" s="15" t="s">
         <v>242</v>
       </c>
       <c r="K82" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>243</v>
       </c>
       <c r="M82" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="N82" s="17" t="s">
         <v>648</v>
       </c>
-      <c r="N82" s="17" t="s">
+      <c r="O82" s="17" t="s">
         <v>649</v>
-      </c>
-      <c r="O82" s="17" t="s">
-        <v>650</v>
       </c>
       <c r="P82" s="15" t="s">
         <v>244</v>
@@ -6660,28 +6660,28 @@
         <v>240</v>
       </c>
       <c r="H83" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="I83" s="15" t="s">
         <v>485</v>
       </c>
-      <c r="I83" s="15" t="s">
+      <c r="J83" s="15" t="s">
         <v>486</v>
       </c>
-      <c r="J83" s="15" t="s">
-        <v>487</v>
-      </c>
       <c r="K83" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L83" s="17" t="s">
+        <v>650</v>
+      </c>
+      <c r="M83" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="M83" s="17" t="s">
+      <c r="N83" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="N83" s="17" t="s">
-        <v>653</v>
-      </c>
       <c r="O83" s="17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="P83" s="15" t="s">
         <v>246</v>
@@ -6719,16 +6719,16 @@
         <v>249</v>
       </c>
       <c r="K84" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>250</v>
       </c>
       <c r="M84" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="O84" s="17" t="s">
         <v>654</v>
-      </c>
-      <c r="O84" s="17" t="s">
-        <v>655</v>
       </c>
       <c r="P84" s="15" t="s">
         <v>251</v>
@@ -6766,19 +6766,19 @@
         <v>254</v>
       </c>
       <c r="K85" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L85" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="M85" s="17" t="s">
         <v>656</v>
-      </c>
-      <c r="M85" s="17" t="s">
-        <v>657</v>
       </c>
       <c r="N85" s="17" t="s">
         <v>316</v>
       </c>
       <c r="O85" s="17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="P85" s="15" t="s">
         <v>255</v>
@@ -6813,22 +6813,22 @@
         <v>253</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K86" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L86" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="M86" s="17" t="s">
         <v>659</v>
       </c>
-      <c r="M86" s="17" t="s">
+      <c r="N86" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="N86" s="17" t="s">
+      <c r="O86" s="17" t="s">
         <v>661</v>
-      </c>
-      <c r="O86" s="17" t="s">
-        <v>662</v>
       </c>
       <c r="P86" s="15" t="s">
         <v>257</v>
@@ -6857,28 +6857,28 @@
         <v>74</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I87" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>127</v>
       </c>
       <c r="K87" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L87" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="M87" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="M87" s="17" t="s">
+      <c r="N87" s="17" t="s">
         <v>664</v>
       </c>
-      <c r="N87" s="17" t="s">
+      <c r="O87" s="17" t="s">
         <v>665</v>
-      </c>
-      <c r="O87" s="17" t="s">
-        <v>666</v>
       </c>
       <c r="P87" s="15" t="s">
         <v>259</v>
@@ -6907,28 +6907,28 @@
         <v>74</v>
       </c>
       <c r="H88" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="I88" s="15" t="s">
         <v>490</v>
-      </c>
-      <c r="I88" s="15" t="s">
-        <v>491</v>
       </c>
       <c r="J88" s="15" t="s">
         <v>127</v>
       </c>
       <c r="K88" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L88" s="17" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M88" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="N88" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="N88" s="17" t="s">
+      <c r="O88" s="17" t="s">
         <v>668</v>
-      </c>
-      <c r="O88" s="17" t="s">
-        <v>669</v>
       </c>
       <c r="P88" s="15" t="s">
         <v>261</v>
@@ -6966,19 +6966,19 @@
         <v>265</v>
       </c>
       <c r="K89" s="17" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L89" s="17" t="s">
+        <v>669</v>
+      </c>
+      <c r="M89" s="17" t="s">
         <v>670</v>
       </c>
-      <c r="M89" s="17" t="s">
+      <c r="N89" s="17" t="s">
         <v>671</v>
       </c>
-      <c r="N89" s="17" t="s">
+      <c r="O89" s="17" t="s">
         <v>672</v>
-      </c>
-      <c r="O89" s="17" t="s">
-        <v>673</v>
       </c>
       <c r="P89" s="15" t="s">
         <v>266</v>
@@ -7016,16 +7016,16 @@
         <v>242</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>313</v>
       </c>
       <c r="M90" s="17" t="s">
+        <v>673</v>
+      </c>
+      <c r="O90" s="17" t="s">
         <v>674</v>
-      </c>
-      <c r="O90" s="17" t="s">
-        <v>675</v>
       </c>
       <c r="P90" s="15" t="s">
         <v>269</v>
@@ -7054,7 +7054,7 @@
         <v>74</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I91" s="15" t="s">
         <v>264</v>
@@ -7063,16 +7063,16 @@
         <v>271</v>
       </c>
       <c r="K91" s="17" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>314</v>
       </c>
       <c r="M91" s="17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O91" s="17" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="P91" s="15" t="s">
         <v>272</v>
@@ -7101,7 +7101,7 @@
         <v>74</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I92" s="15" t="s">
         <v>268</v>
@@ -7110,19 +7110,19 @@
         <v>271</v>
       </c>
       <c r="K92" s="17" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="L92" s="17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="M92" s="15" t="s">
         <v>274</v>
       </c>
       <c r="N92" s="17" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O92" s="17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="P92" s="15" t="s">
         <v>275</v>
@@ -7151,7 +7151,7 @@
         <v>74</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I93" s="15" t="s">
         <v>264</v>
@@ -7160,19 +7160,19 @@
         <v>277</v>
       </c>
       <c r="K93" s="17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>278</v>
       </c>
       <c r="M93" s="17" t="s">
+        <v>677</v>
+      </c>
+      <c r="N93" s="17" t="s">
         <v>678</v>
       </c>
-      <c r="N93" s="17" t="s">
-        <v>679</v>
-      </c>
       <c r="O93" s="17" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="P93" s="15" t="s">
         <v>279</v>
@@ -7201,28 +7201,28 @@
         <v>74</v>
       </c>
       <c r="H94" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="I94" s="15" t="s">
         <v>494</v>
       </c>
-      <c r="I94" s="15" t="s">
+      <c r="J94" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="J94" s="15" t="s">
-        <v>496</v>
-      </c>
       <c r="K94" s="17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="L94" s="17" t="s">
+        <v>679</v>
+      </c>
+      <c r="M94" s="17" t="s">
         <v>680</v>
       </c>
-      <c r="M94" s="17" t="s">
+      <c r="N94" s="17" t="s">
         <v>681</v>
       </c>
-      <c r="N94" s="17" t="s">
+      <c r="O94" s="17" t="s">
         <v>682</v>
-      </c>
-      <c r="O94" s="17" t="s">
-        <v>683</v>
       </c>
       <c r="P94" s="15" t="s">
         <v>281</v>
@@ -7257,22 +7257,22 @@
         <v>283</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K95" s="17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L95" s="17" t="s">
+        <v>683</v>
+      </c>
+      <c r="M95" s="17" t="s">
         <v>684</v>
       </c>
-      <c r="M95" s="17" t="s">
+      <c r="N95" s="17" t="s">
         <v>685</v>
       </c>
-      <c r="N95" s="17" t="s">
+      <c r="O95" s="17" t="s">
         <v>686</v>
-      </c>
-      <c r="O95" s="17" t="s">
-        <v>687</v>
       </c>
       <c r="P95" s="15" t="s">
         <v>284</v>
@@ -7310,16 +7310,16 @@
         <v>242</v>
       </c>
       <c r="K96" s="17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="L96" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="M96" s="17" t="s">
         <v>688</v>
       </c>
-      <c r="M96" s="17" t="s">
-        <v>689</v>
-      </c>
       <c r="O96" s="17" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P96" s="15" t="s">
         <v>286</v>
@@ -7357,19 +7357,19 @@
         <v>242</v>
       </c>
       <c r="K97" s="17" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>290</v>
       </c>
       <c r="M97" s="17" t="s">
+        <v>689</v>
+      </c>
+      <c r="N97" s="17" t="s">
         <v>690</v>
       </c>
-      <c r="N97" s="17" t="s">
+      <c r="O97" s="17" t="s">
         <v>691</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>692</v>
       </c>
       <c r="P97" s="15" t="s">
         <v>291</v>
@@ -7398,28 +7398,28 @@
         <v>293</v>
       </c>
       <c r="H98" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="I98" s="15" t="s">
         <v>498</v>
-      </c>
-      <c r="I98" s="15" t="s">
-        <v>499</v>
       </c>
       <c r="J98" s="15" t="s">
         <v>294</v>
       </c>
       <c r="K98" s="17" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="L98" s="15" t="s">
         <v>295</v>
       </c>
       <c r="M98" s="17" t="s">
+        <v>692</v>
+      </c>
+      <c r="N98" s="17" t="s">
         <v>693</v>
       </c>
-      <c r="N98" s="17" t="s">
+      <c r="O98" s="17" t="s">
         <v>694</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>695</v>
       </c>
       <c r="P98" s="15" t="s">
         <v>296</v>
@@ -7448,28 +7448,28 @@
         <v>74</v>
       </c>
       <c r="H99" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="I99" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="I99" s="15" t="s">
+      <c r="J99" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="J99" s="15" t="s">
-        <v>502</v>
-      </c>
       <c r="K99" s="17" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="L99" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="M99" s="17" t="s">
         <v>696</v>
       </c>
-      <c r="M99" s="17" t="s">
+      <c r="N99" s="17" t="s">
         <v>697</v>
       </c>
-      <c r="N99" s="17" t="s">
+      <c r="O99" s="17" t="s">
         <v>698</v>
-      </c>
-      <c r="O99" s="17" t="s">
-        <v>699</v>
       </c>
       <c r="P99" s="15" t="s">
         <v>298</v>
@@ -7498,28 +7498,28 @@
         <v>293</v>
       </c>
       <c r="H100" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="I100" s="15" t="s">
         <v>498</v>
-      </c>
-      <c r="I100" s="15" t="s">
-        <v>499</v>
       </c>
       <c r="J100" s="15" t="s">
         <v>300</v>
       </c>
       <c r="K100" s="17" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L100" s="17" t="s">
+        <v>699</v>
+      </c>
+      <c r="M100" s="17" t="s">
         <v>700</v>
       </c>
-      <c r="M100" s="17" t="s">
+      <c r="N100" s="17" t="s">
         <v>701</v>
       </c>
-      <c r="N100" s="17" t="s">
+      <c r="O100" s="17" t="s">
         <v>702</v>
-      </c>
-      <c r="O100" s="17" t="s">
-        <v>703</v>
       </c>
       <c r="P100" s="15" t="s">
         <v>301</v>
@@ -7557,16 +7557,16 @@
         <v>305</v>
       </c>
       <c r="K101" s="17" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="L101" s="15" t="s">
         <v>315</v>
       </c>
       <c r="M101" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="O101" s="17" t="s">
         <v>704</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>705</v>
       </c>
       <c r="P101" s="15" t="s">
         <v>306</v>
@@ -7781,18 +7781,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7814,14 +7814,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FC7F45C-4F37-4DFF-BDAF-78C0D0B5C911}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{416110E1-8220-4910-BAF6-7757097D35BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -7835,4 +7827,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FC7F45C-4F37-4DFF-BDAF-78C0D0B5C911}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes to Revision. Simplified cuisine field to only have one type. Added fusion and hokkien to ontology.
</commit_message>
<xml_diff>
--- a/recipeData/CombineRecipes.xlsx
+++ b/recipeData/CombineRecipes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="772">
   <si>
     <t>Name</t>
   </si>
@@ -1001,9 +1001,6 @@
     <t>dried shrimps;Nyonya Sambal chilly;fine sugar;lime leaves</t>
   </si>
   <si>
-    <t>Asian; Indonesian; Nonya; Vegetarian</t>
-  </si>
-  <si>
     <t>Appetizer; Snack</t>
   </si>
   <si>
@@ -1016,15 +1013,9 @@
     <t>vegetarian chicken;cooking oil;glutinous rice;blue pea flower;hemp string;pandan leaves;salt;dried bamboo leaves;biryani powder;water;mushroom stock;brown sugar;winter melon;dried chilly;lemongrass;blue ginger;turmeric</t>
   </si>
   <si>
-    <t>Asian; Vegetarian</t>
-  </si>
-  <si>
     <t>yellow capsicums;cooked rice;French beans;canned corn kernels;tomato;extra virgin olive oil; Salt;pepper;coriander;shredded cheese</t>
   </si>
   <si>
-    <t>Chinese; Asian; Nyonya; Peranakan</t>
-  </si>
-  <si>
     <t>chicken;meat curry powder;chilly powder;cooking oil;potato;water;curry leaf;coconut milk;tamarind peel;salt2 stalks lemon grass;cinnamon stick;anise;cardamon;shallots;garlic;ginger</t>
   </si>
   <si>
@@ -1049,9 +1040,6 @@
     <t>yam bean;guava;cucumber;carrot;green papaya;pomelo sac;rice flour;tapioca flour;egg;water;salt;sugar;small prawn;galangal;bird’s eye chilly;fresh red chilly;plum sauce;salt;cooking oil;crushed fried peanuts;toasted sesame seeds</t>
   </si>
   <si>
-    <t>Asian; Indonesian; Nyonya; Peranakan</t>
-  </si>
-  <si>
     <t>Fish; Seafood</t>
   </si>
   <si>
@@ -1064,18 +1052,12 @@
     <t>spring roll wrappers;flour;cooking oil;curry Leaves;mustard seed;cumin; garlic;onion; fish curry powder; pumpkin; water; green peas; coconut milk; sugar; salt</t>
   </si>
   <si>
-    <t>Asian; Nyonya; Peranakan; Vegetarian</t>
-  </si>
-  <si>
     <t>Vegetable; Fruit</t>
   </si>
   <si>
     <t>cooking oil;cinnamon stick;star anise;clove;shallot;garlic;fish curry powder;water;tamarind paste;palm sugar;pineapple;coconut milk;salt</t>
   </si>
   <si>
-    <t>Asian; Chinese; Nyonya</t>
-  </si>
-  <si>
     <t>Chicken; Pork</t>
   </si>
   <si>
@@ -1088,9 +1070,6 @@
     <t>cooking oil;shallots;garlic;shallot;soya bean paste;prawn;chicken;yellow egg noodles;mustard green;bean sprout;water;dark soya sauce;light soya sauce;sugar;white pepper;Salt;fresh red chilly;red chilly padi;belachan;shallot crisp</t>
   </si>
   <si>
-    <t>Asian; Malaysia; Nyonya</t>
-  </si>
-  <si>
     <t>cooking oil;onion;chicken;brown sugar;kaffir lime leave;water;coconut milk;lime juice;Salt;shallot;garlic;ginger;galangal;turmeric;candle nut;lemon grass;dried chilly;bird’s eye chilly;belachan</t>
   </si>
   <si>
@@ -1100,15 +1079,9 @@
     <t>glutinous rice;dried prawns;lean pork;candied winter melon;lemon grass;knob galangal;dried chilly;garlic;shallot;coriander seed;sugar;Blue pea flowers;pandan leave</t>
   </si>
   <si>
-    <t>Asian; Chinese; Vegetarian</t>
-  </si>
-  <si>
     <t>hard tofu;sweet corn kernel;red bell pepper;snow pea pod;chilly paste;shallot;garlic;honey;salt</t>
   </si>
   <si>
-    <t>Asian; Indonesian; Nonya; Peranakan</t>
-  </si>
-  <si>
     <t>Noodle; Pork; Vegetable</t>
   </si>
   <si>
@@ -1121,9 +1094,6 @@
     <t>chicken drummets;ginger juice; corn flour;chilly flakes;oyster sauce; chicken stock granules; dark soya sauce;lime leaves;honey;salt</t>
   </si>
   <si>
-    <t>Asian; Peranakan; Nyonya</t>
-  </si>
-  <si>
     <t>Vegetable; Turkey</t>
   </si>
   <si>
@@ -1139,27 +1109,18 @@
     <t>sweet potato flesh;coarse sugar;water;tapioca flour;thick coconut milk;salt;coconut flesh</t>
   </si>
   <si>
-    <t>Nyonya; Asian; Peranakan; Malaysia</t>
-  </si>
-  <si>
     <t>stir frying; Boiling</t>
   </si>
   <si>
     <t>glutinous rice;freshly ground turmeric;tamarind peel;pepper corn;salt;dried bamboo leave;hemp string;cooking oil;dried chilly;shallot;sugar;salt;dried prawn</t>
   </si>
   <si>
-    <t>Asian; Nyonya; Peranakan</t>
-  </si>
-  <si>
     <t>Grill; Boiling</t>
   </si>
   <si>
     <t>pork belly;tamarind paste;water;salt;sugar</t>
   </si>
   <si>
-    <t>Asian; Chinese</t>
-  </si>
-  <si>
     <t>Wok; claypot</t>
   </si>
   <si>
@@ -1172,9 +1133,6 @@
     <t>skinless chicken breast;chicken drumsticks;rice;corn oil;ginger;scallion;mushroom;oyster sauce;soy sauce;corn starch;sesame oil;white pepper;sugar;shaoxing wine;dark soy sauce;salt</t>
   </si>
   <si>
-    <t>Asian; Malay/Indonesian</t>
-  </si>
-  <si>
     <t>noodle; seafood;pork</t>
   </si>
   <si>
@@ -1184,9 +1142,6 @@
     <t>black pepper;melted unsalted butter;garlic;onion;crab;oyster sauce;sugar;water;salt</t>
   </si>
   <si>
-    <t>Asian; Singaporean</t>
-  </si>
-  <si>
     <t>pork; vegetable</t>
   </si>
   <si>
@@ -1202,15 +1157,9 @@
     <t>claim; onion;garlic;vegetable oil;chinese rice wine;ginger;chilies;sasame oil;spring onion;light soya sauce</t>
   </si>
   <si>
-    <t>Chinese; Asian</t>
-  </si>
-  <si>
     <t>prawn;butter;salt;pepper</t>
   </si>
   <si>
-    <t>Asian; chinese</t>
-  </si>
-  <si>
     <t>fish;rice</t>
   </si>
   <si>
@@ -1226,9 +1175,6 @@
     <t>cod fillet;salt;white pepper;tomato;sour plum;silken tofu;ginger;cooking oil;garlic;pork;preserved mustard;water;soy sauce;shaoxing wine;sugar;onion;coriander</t>
   </si>
   <si>
-    <t>asian;chinese;hokkien</t>
-  </si>
-  <si>
     <t>breakfast;brunch;easy</t>
   </si>
   <si>
@@ -1262,9 +1208,6 @@
     <t>butter;cooking oil;shallot;eye chilies;bird eye chilies;curry leave;salted egg yolk;evaporated milk;water;prawn;sugar;salt</t>
   </si>
   <si>
-    <t>asian;singaporean</t>
-  </si>
-  <si>
     <t>stir frying/wok;boiling/double boiling</t>
   </si>
   <si>
@@ -1280,9 +1223,6 @@
     <t>confectioner sugar;flour;egg;butter;dash vanilla;sugar;water;evaporated milk</t>
   </si>
   <si>
-    <t>Indian; Asian</t>
-  </si>
-  <si>
     <t>Boiling; low heat and simmer</t>
   </si>
   <si>
@@ -1334,9 +1274,6 @@
     <t>Tandoori Chicken; butter; finely minced ginger; finely minced garlic; canned tomato paste; chili powder; Garam Masala; ketchup; teaspoon sugar; Salt; water; heavy whipped cream; cilantro leaves</t>
   </si>
   <si>
-    <t>Indian; Asian; Vegetarian</t>
-  </si>
-  <si>
     <t>Cauliflower; Potatoes</t>
   </si>
   <si>
@@ -1349,9 +1286,6 @@
     <t>Blender; Pot</t>
   </si>
   <si>
-    <t>Indian; Asian; Italian</t>
-  </si>
-  <si>
     <t>Stir Fry; Oven bake</t>
   </si>
   <si>
@@ -1373,18 +1307,12 @@
     <t>rie firm green mango; cinnamon; cloves; cumin seeds; coriander seeds; cardamom; ginger; dry red chilly; garlic; demerara suga; vinegar; water; salt</t>
   </si>
   <si>
-    <t>Western; European; French</t>
-  </si>
-  <si>
     <t>Oven;Piping bag;Plain nozzle</t>
   </si>
   <si>
     <t xml:space="preserve">almonds; icing sugar; aged egg whites; caster sugar; pink food colouring powder; rose essence                                                                                                                                            </t>
   </si>
   <si>
-    <t>Asian; Malaysia; Nonya/Peranakan</t>
-  </si>
-  <si>
     <t>food processor;frying pan</t>
   </si>
   <si>
@@ -1403,9 +1331,6 @@
     <t>Oil ; chicken; garlic powder; salt;ground turmeric ; ground nutmeg; butter</t>
   </si>
   <si>
-    <t>Western; American</t>
-  </si>
-  <si>
     <t>red onions; red bell pepper; large red chilli; honey red tomatoes; bulb garlic; stick cinnamon; fish sauce; sugar; oil</t>
   </si>
   <si>
@@ -2375,15 +2300,6 @@
     <t>cherry tomatoes</t>
   </si>
   <si>
-    <t>Nyonya; Asian; Singapore; Malay</t>
-  </si>
-  <si>
-    <t>Asian; Indian; Vegetarian</t>
-  </si>
-  <si>
-    <t>Asian; Malay; Indonesian</t>
-  </si>
-  <si>
     <t>Chinese</t>
   </si>
   <si>
@@ -2400,6 +2316,30 @@
   </si>
   <si>
     <t>Oven;Brass moulds</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Peranakan</t>
+  </si>
+  <si>
+    <t>Singaporean</t>
+  </si>
+  <si>
+    <t>Hokkien</t>
+  </si>
+  <si>
+    <t>Fusion</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Malay</t>
+  </si>
+  <si>
+    <t>American</t>
   </si>
 </sst>
 </file>
@@ -2826,8 +2766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2835,6 +2775,7 @@
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="9" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
@@ -2912,7 +2853,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>783</v>
+        <v>29</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>15</v>
@@ -2930,12 +2871,12 @@
         <v>324</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="17" t="s">
-        <v>503</v>
+        <v>478</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>17</v>
@@ -2958,32 +2899,32 @@
         <v>135</v>
       </c>
       <c r="F3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>325</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>326</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>81</v>
       </c>
       <c r="I3" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>329</v>
-      </c>
       <c r="L3" s="17" t="s">
-        <v>504</v>
+        <v>479</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="17" t="s">
-        <v>712</v>
+        <v>687</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>19</v>
@@ -3006,7 +2947,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>330</v>
+        <v>37</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>74</v>
@@ -3018,18 +2959,18 @@
         <v>307</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="17" t="s">
-        <v>507</v>
+        <v>482</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>22</v>
@@ -3052,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>332</v>
+        <v>29</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>74</v>
@@ -3067,17 +3008,17 @@
         <v>24</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>508</v>
+        <v>483</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>509</v>
+        <v>484</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="17" t="s">
-        <v>510</v>
+        <v>485</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>25</v>
@@ -3100,7 +3041,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>374</v>
+        <v>29</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>74</v>
@@ -3109,23 +3050,23 @@
         <v>81</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>511</v>
+        <v>486</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>512</v>
+        <v>487</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="17" t="s">
-        <v>513</v>
+        <v>488</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>27</v>
@@ -3157,23 +3098,23 @@
         <v>90</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>759</v>
+        <v>734</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>514</v>
+        <v>489</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>515</v>
+        <v>490</v>
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="17" t="s">
-        <v>721</v>
+        <v>696</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>30</v>
@@ -3211,12 +3152,12 @@
         <v>34</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>516</v>
+        <v>491</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="17" t="s">
-        <v>517</v>
+        <v>492</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>35</v>
@@ -3251,22 +3192,22 @@
         <v>309</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>518</v>
+        <v>493</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>519</v>
+        <v>494</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>520</v>
+        <v>495</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>521</v>
+        <v>496</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>39</v>
@@ -3289,10 +3230,10 @@
         <v>30</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>341</v>
+        <v>29</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>789</v>
+        <v>761</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>90</v>
@@ -3301,20 +3242,20 @@
         <v>308</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>522</v>
+        <v>497</v>
       </c>
       <c r="M10" s="15" t="s">
         <v>41</v>
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="17" t="s">
-        <v>523</v>
+        <v>498</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>42</v>
@@ -3337,10 +3278,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>784</v>
+        <v>764</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>788</v>
+        <v>760</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>81</v>
@@ -3352,17 +3293,17 @@
         <v>45</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>524</v>
+        <v>499</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>525</v>
+        <v>500</v>
       </c>
       <c r="N11" s="15"/>
       <c r="O11" s="17" t="s">
-        <v>526</v>
+        <v>501</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>46</v>
@@ -3385,7 +3326,7 @@
         <v>140</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>346</v>
+        <v>29</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>74</v>
@@ -3397,18 +3338,18 @@
         <v>309</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>527</v>
+        <v>502</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="17" t="s">
-        <v>722</v>
+        <v>697</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>48</v>
@@ -3431,7 +3372,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>349</v>
+        <v>29</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>74</v>
@@ -3443,20 +3384,20 @@
         <v>309</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>528</v>
+        <v>503</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>529</v>
+        <v>504</v>
       </c>
       <c r="N13" s="15"/>
       <c r="O13" s="17" t="s">
-        <v>723</v>
+        <v>698</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>50</v>
@@ -3479,7 +3420,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>349</v>
+        <v>29</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>74</v>
@@ -3491,22 +3432,22 @@
         <v>309</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>530</v>
+        <v>505</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>531</v>
+        <v>506</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>319</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>724</v>
+        <v>699</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>52</v>
@@ -3529,7 +3470,7 @@
         <v>30</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>354</v>
+        <v>29</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>74</v>
@@ -3544,17 +3485,17 @@
         <v>24</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>532</v>
+        <v>507</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>533</v>
+        <v>508</v>
       </c>
       <c r="N15" s="15"/>
       <c r="O15" s="17" t="s">
-        <v>725</v>
+        <v>700</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>54</v>
@@ -3577,10 +3518,10 @@
         <v>250</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>349</v>
+        <v>29</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H16" s="15" t="s">
         <v>90</v>
@@ -3589,18 +3530,18 @@
         <v>310</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>534</v>
+        <v>509</v>
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="17" t="s">
-        <v>726</v>
+        <v>701</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>56</v>
@@ -3623,7 +3564,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>358</v>
+        <v>758</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>74</v>
@@ -3635,20 +3576,20 @@
         <v>309</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>535</v>
+        <v>510</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>536</v>
+        <v>511</v>
       </c>
       <c r="N17" s="15"/>
       <c r="O17" s="17" t="s">
-        <v>727</v>
+        <v>702</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>58</v>
@@ -3671,7 +3612,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>360</v>
+        <v>765</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>74</v>
@@ -3683,18 +3624,18 @@
         <v>33</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>537</v>
+        <v>512</v>
       </c>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="17" t="s">
-        <v>728</v>
+        <v>703</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>60</v>
@@ -3717,7 +3658,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>354</v>
+        <v>29</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>74</v>
@@ -3726,21 +3667,21 @@
         <v>288</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="J19" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>538</v>
+        <v>513</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="15"/>
       <c r="O19" s="17" t="s">
-        <v>729</v>
+        <v>704</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>62</v>
@@ -3763,7 +3704,7 @@
         <v>120</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>365</v>
+        <v>765</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>74</v>
@@ -3775,18 +3716,18 @@
         <v>96</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>539</v>
+        <v>514</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="15"/>
       <c r="O20" s="17" t="s">
-        <v>730</v>
+        <v>705</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>64</v>
@@ -3809,13 +3750,13 @@
         <v>300</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>349</v>
+        <v>29</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>310</v>
@@ -3824,15 +3765,15 @@
         <v>45</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>540</v>
+        <v>515</v>
       </c>
       <c r="M21" s="17"/>
       <c r="N21" s="15"/>
       <c r="O21" s="17" t="s">
-        <v>731</v>
+        <v>706</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>66</v>
@@ -3840,7 +3781,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>705</v>
+        <v>680</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>322</v>
@@ -3855,32 +3796,32 @@
         <v>135</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>371</v>
+        <v>29</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>788</v>
+        <v>760</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>81</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>67</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>541</v>
+        <v>516</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>542</v>
+        <v>517</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="17" t="s">
-        <v>732</v>
+        <v>707</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>68</v>
@@ -3902,8 +3843,8 @@
       <c r="E23" s="22">
         <v>50</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>374</v>
+      <c r="F23" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>74</v>
@@ -3912,20 +3853,20 @@
         <v>288</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="J23" s="22" t="s">
         <v>70</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>543</v>
+        <v>518</v>
       </c>
       <c r="M23" s="24"/>
       <c r="O23" s="24" t="s">
-        <v>733</v>
+        <v>708</v>
       </c>
       <c r="P23" s="25" t="s">
         <v>71</v>
@@ -3947,32 +3888,32 @@
       <c r="E24" s="22">
         <v>30</v>
       </c>
-      <c r="F24" s="22" t="s">
-        <v>377</v>
+      <c r="F24" s="15" t="s">
+        <v>758</v>
       </c>
       <c r="G24" s="22" t="s">
         <v>74</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>544</v>
+        <v>519</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>546</v>
+        <v>521</v>
       </c>
       <c r="P24" s="25" t="s">
         <v>75</v>
@@ -3995,31 +3936,31 @@
         <v>60</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>785</v>
+        <v>218</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>547</v>
+        <v>522</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>548</v>
+        <v>523</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>549</v>
+        <v>524</v>
       </c>
       <c r="P25" s="15" t="s">
         <v>78</v>
@@ -4042,7 +3983,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>386</v>
+        <v>766</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>80</v>
@@ -4057,13 +3998,13 @@
         <v>83</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>551</v>
+        <v>526</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>84</v>
@@ -4086,7 +4027,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>386</v>
+        <v>766</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>80</v>
@@ -4098,16 +4039,16 @@
         <v>86</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>552</v>
+        <v>527</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="P27" s="15" t="s">
         <v>87</v>
@@ -4142,16 +4083,16 @@
         <v>91</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>555</v>
+        <v>530</v>
       </c>
       <c r="P28" s="15" t="s">
         <v>92</v>
@@ -4159,7 +4100,7 @@
     </row>
     <row r="29" spans="1:16" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>790</v>
+        <v>762</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>320</v>
@@ -4174,7 +4115,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>377</v>
+        <v>758</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>74</v>
@@ -4189,13 +4130,13 @@
         <v>83</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>556</v>
+        <v>531</v>
       </c>
       <c r="O29" s="17" t="s">
-        <v>557</v>
+        <v>532</v>
       </c>
       <c r="P29" s="15" t="s">
         <v>94</v>
@@ -4218,7 +4159,7 @@
         <v>15</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>74</v>
@@ -4233,16 +4174,16 @@
         <v>83</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>558</v>
+        <v>533</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>734</v>
+        <v>709</v>
       </c>
       <c r="P30" s="15" t="s">
         <v>97</v>
@@ -4265,7 +4206,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>394</v>
+        <v>758</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>74</v>
@@ -4277,16 +4218,16 @@
         <v>99</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>560</v>
+        <v>535</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>561</v>
+        <v>536</v>
       </c>
       <c r="P31" s="15" t="s">
         <v>100</v>
@@ -4309,7 +4250,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>74</v>
@@ -4318,25 +4259,25 @@
         <v>81</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>562</v>
+        <v>537</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>563</v>
+        <v>538</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>564</v>
+        <v>539</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>565</v>
+        <v>540</v>
       </c>
       <c r="P32" s="15" t="s">
         <v>102</v>
@@ -4359,28 +4300,28 @@
         <v>55</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>400</v>
+        <v>767</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>81</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="J33" s="15" t="s">
         <v>104</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>566</v>
+        <v>541</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="P33" s="15" t="s">
         <v>105</v>
@@ -4403,7 +4344,7 @@
         <v>8</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>74</v>
@@ -4418,13 +4359,13 @@
         <v>83</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="O34" s="17" t="s">
-        <v>569</v>
+        <v>544</v>
       </c>
       <c r="P34" s="15" t="s">
         <v>108</v>
@@ -4447,7 +4388,7 @@
         <v>250</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>74</v>
@@ -4459,16 +4400,16 @@
         <v>107</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>570</v>
+        <v>545</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>571</v>
+        <v>546</v>
       </c>
       <c r="P35" s="15" t="s">
         <v>110</v>
@@ -4491,7 +4432,7 @@
         <v>10</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G36" s="15" t="s">
         <v>74</v>
@@ -4506,13 +4447,13 @@
         <v>112</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>572</v>
+        <v>547</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>573</v>
+        <v>548</v>
       </c>
       <c r="P36" s="15" t="s">
         <v>113</v>
@@ -4535,7 +4476,7 @@
         <v>12</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>74</v>
@@ -4550,13 +4491,13 @@
         <v>112</v>
       </c>
       <c r="K37" s="17" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>574</v>
+        <v>549</v>
       </c>
       <c r="O37" s="17" t="s">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="P37" s="15" t="s">
         <v>115</v>
@@ -4579,7 +4520,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>74</v>
@@ -4594,13 +4535,13 @@
         <v>117</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>576</v>
+        <v>551</v>
       </c>
       <c r="O38" s="17" t="s">
-        <v>577</v>
+        <v>552</v>
       </c>
       <c r="P38" s="15" t="s">
         <v>118</v>
@@ -4623,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>74</v>
@@ -4635,16 +4576,16 @@
         <v>107</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="L39" s="17" t="s">
-        <v>578</v>
+        <v>553</v>
       </c>
       <c r="M39" s="17" t="s">
-        <v>579</v>
+        <v>554</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="P39" s="15" t="s">
         <v>120</v>
@@ -4667,7 +4608,7 @@
         <v>8</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>392</v>
+        <v>758</v>
       </c>
       <c r="G40" s="15" t="s">
         <v>74</v>
@@ -4682,13 +4623,13 @@
         <v>83</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>706</v>
+        <v>681</v>
       </c>
       <c r="P40" s="15" t="s">
         <v>122</v>
@@ -4711,7 +4652,7 @@
         <v>30</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>412</v>
+        <v>766</v>
       </c>
       <c r="G41" s="15" t="s">
         <v>89</v>
@@ -4720,19 +4661,19 @@
         <v>90</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>582</v>
+        <v>557</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="P41" s="15" t="s">
         <v>124</v>
@@ -4755,7 +4696,7 @@
         <v>15</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>786</v>
+        <v>758</v>
       </c>
       <c r="G42" s="15" t="s">
         <v>74</v>
@@ -4770,13 +4711,13 @@
         <v>127</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>585</v>
+        <v>560</v>
       </c>
       <c r="P42" s="15" t="s">
         <v>128</v>
@@ -4799,7 +4740,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>786</v>
+        <v>758</v>
       </c>
       <c r="G43" s="15" t="s">
         <v>130</v>
@@ -4811,13 +4752,13 @@
         <v>131</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>707</v>
+        <v>682</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>708</v>
+        <v>683</v>
       </c>
       <c r="P43" s="15" t="s">
         <v>132</v>
@@ -4840,7 +4781,7 @@
         <v>20</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>74</v>
@@ -4849,21 +4790,21 @@
         <v>134</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>586</v>
+        <v>561</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>587</v>
+        <v>562</v>
       </c>
       <c r="P44" s="4" t="s">
         <v>135</v>
@@ -4886,7 +4827,7 @@
         <v>30</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G45" s="22" t="s">
         <v>74</v>
@@ -4901,15 +4842,15 @@
         <v>24</v>
       </c>
       <c r="K45" s="17" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="L45" s="17" t="s">
-        <v>588</v>
+        <v>563</v>
       </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17" t="s">
-        <v>589</v>
+        <v>564</v>
       </c>
       <c r="P45" s="4" t="s">
         <v>139</v>
@@ -4932,7 +4873,7 @@
         <v>20</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G46" s="22" t="s">
         <v>74</v>
@@ -4941,21 +4882,21 @@
         <v>141</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>590</v>
+        <v>565</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17" t="s">
-        <v>735</v>
+        <v>710</v>
       </c>
       <c r="P46" s="4" t="s">
         <v>142</v>
@@ -4978,7 +4919,7 @@
         <v>15</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G47" s="22" t="s">
         <v>74</v>
@@ -4993,15 +4934,15 @@
         <v>146</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="L47" s="17" t="s">
-        <v>591</v>
+        <v>566</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
       <c r="O47" s="17" t="s">
-        <v>736</v>
+        <v>711</v>
       </c>
       <c r="P47" s="4" t="s">
         <v>147</v>
@@ -5024,7 +4965,7 @@
         <v>40</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G48" s="22" t="s">
         <v>74</v>
@@ -5039,15 +4980,15 @@
         <v>24</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="L48" s="17" t="s">
-        <v>592</v>
+        <v>567</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
       <c r="O48" s="17" t="s">
-        <v>593</v>
+        <v>568</v>
       </c>
       <c r="P48" s="4" t="s">
         <v>150</v>
@@ -5070,30 +5011,30 @@
         <v>20</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G49" s="15" t="s">
         <v>152</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>153</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>594</v>
+        <v>569</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17" t="s">
-        <v>718</v>
+        <v>693</v>
       </c>
       <c r="P49" s="4" t="s">
         <v>154</v>
@@ -5116,7 +5057,7 @@
         <v>20</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G50" s="15" t="s">
         <v>156</v>
@@ -5128,18 +5069,18 @@
         <v>157</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="L50" s="17" t="s">
-        <v>595</v>
+        <v>570</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="P50" s="4" t="s">
         <v>158</v>
@@ -5162,7 +5103,7 @@
         <v>10</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G51" s="15" t="s">
         <v>156</v>
@@ -5177,15 +5118,15 @@
         <v>161</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
       <c r="L51" s="17" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="17" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="P51" s="4" t="s">
         <v>162</v>
@@ -5208,7 +5149,7 @@
         <v>10</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G52" s="22" t="s">
         <v>74</v>
@@ -5223,15 +5164,15 @@
         <v>164</v>
       </c>
       <c r="K52" s="17" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="L52" s="17" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
       <c r="O52" s="17" t="s">
-        <v>737</v>
+        <v>712</v>
       </c>
       <c r="P52" s="4" t="s">
         <v>165</v>
@@ -5254,30 +5195,30 @@
         <v>30</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G53" s="22" t="s">
         <v>74</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K53" s="17" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="L53" s="17" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
       <c r="O53" s="17" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="P53" s="4" t="s">
         <v>167</v>
@@ -5300,30 +5241,30 @@
         <v>30</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>436</v>
+        <v>764</v>
       </c>
       <c r="G54" s="22" t="s">
         <v>74</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="J54" s="15" t="s">
         <v>169</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
       <c r="L54" s="17" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
       <c r="O54" s="17" t="s">
-        <v>738</v>
+        <v>713</v>
       </c>
       <c r="P54" s="4" t="s">
         <v>170</v>
@@ -5346,7 +5287,7 @@
         <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>436</v>
+        <v>764</v>
       </c>
       <c r="G55" s="15" t="s">
         <v>172</v>
@@ -5358,18 +5299,18 @@
         <v>138</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>760</v>
+        <v>735</v>
       </c>
       <c r="L55" s="17" t="s">
-        <v>713</v>
+        <v>688</v>
       </c>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
       <c r="O55" s="17" t="s">
-        <v>739</v>
+        <v>714</v>
       </c>
       <c r="P55" s="4" t="s">
         <v>174</v>
@@ -5392,7 +5333,7 @@
         <v>20</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G56" s="22" t="s">
         <v>74</v>
@@ -5407,15 +5348,15 @@
         <v>16</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>761</v>
+        <v>736</v>
       </c>
       <c r="L56" s="17" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
       <c r="O56" s="17" t="s">
-        <v>740</v>
+        <v>715</v>
       </c>
       <c r="P56" s="4" t="s">
         <v>177</v>
@@ -5438,7 +5379,7 @@
         <v>30</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>74</v>
@@ -5453,15 +5394,15 @@
         <v>24</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="L57" s="17" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
       <c r="O57" s="17" t="s">
-        <v>741</v>
+        <v>716</v>
       </c>
       <c r="P57" s="4" t="s">
         <v>180</v>
@@ -5484,13 +5425,13 @@
         <v>40</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>74</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="I58" s="15" t="s">
         <v>153</v>
@@ -5499,15 +5440,15 @@
         <v>24</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="L58" s="17" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17" t="s">
-        <v>742</v>
+        <v>717</v>
       </c>
       <c r="P58" s="4" t="s">
         <v>182</v>
@@ -5530,30 +5471,30 @@
         <v>20</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>441</v>
+        <v>768</v>
       </c>
       <c r="G59" s="22" t="s">
         <v>74</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>442</v>
+        <v>420</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>443</v>
+        <v>421</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>762</v>
+        <v>737</v>
       </c>
       <c r="L59" s="17" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
       <c r="O59" s="17" t="s">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="P59" s="4" t="s">
         <v>184</v>
@@ -5576,7 +5517,7 @@
         <v>30</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G60" s="22" t="s">
         <v>74</v>
@@ -5591,15 +5532,15 @@
         <v>24</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>763</v>
+        <v>738</v>
       </c>
       <c r="L60" s="17" t="s">
-        <v>608</v>
+        <v>583</v>
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
       <c r="O60" s="17" t="s">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="P60" s="4" t="s">
         <v>186</v>
@@ -5622,10 +5563,10 @@
         <v>10</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>787</v>
+        <v>759</v>
       </c>
       <c r="H61" s="15" t="s">
         <v>188</v>
@@ -5637,15 +5578,15 @@
         <v>146</v>
       </c>
       <c r="K61" s="17" t="s">
-        <v>764</v>
+        <v>739</v>
       </c>
       <c r="L61" s="17" t="s">
-        <v>610</v>
+        <v>585</v>
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
       <c r="O61" s="17" t="s">
-        <v>611</v>
+        <v>586</v>
       </c>
       <c r="P61" s="4" t="s">
         <v>189</v>
@@ -5668,10 +5609,10 @@
         <v>45</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>418</v>
+        <v>764</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="H62" s="15" t="s">
         <v>191</v>
@@ -5680,18 +5621,18 @@
         <v>153</v>
       </c>
       <c r="J62" s="15" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="K62" s="17" t="s">
-        <v>765</v>
+        <v>740</v>
       </c>
       <c r="L62" s="17" t="s">
-        <v>612</v>
+        <v>587</v>
       </c>
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
       <c r="O62" s="17" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="P62" s="4" t="s">
         <v>192</v>
@@ -5714,13 +5655,13 @@
         <v>30</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>449</v>
+        <v>769</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>32</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="I63" s="11" t="s">
         <v>21</v>
@@ -5729,17 +5670,17 @@
         <v>194</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>766</v>
+        <v>741</v>
       </c>
       <c r="L63" s="20" t="s">
-        <v>614</v>
+        <v>589</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>615</v>
+        <v>590</v>
       </c>
       <c r="N63" s="11"/>
       <c r="O63" s="20" t="s">
-        <v>743</v>
+        <v>718</v>
       </c>
       <c r="P63" s="11" t="s">
         <v>195</v>
@@ -5762,32 +5703,32 @@
         <v>30</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>452</v>
+        <v>29</v>
       </c>
       <c r="G64" s="11" t="s">
         <v>197</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="J64" s="11" t="s">
         <v>24</v>
       </c>
       <c r="K64" s="11" t="s">
-        <v>767</v>
+        <v>742</v>
       </c>
       <c r="L64" s="20" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>617</v>
+        <v>592</v>
       </c>
       <c r="N64" s="11"/>
       <c r="O64" s="20" t="s">
-        <v>618</v>
+        <v>593</v>
       </c>
       <c r="P64" s="11" t="s">
         <v>198</v>
@@ -5825,19 +5766,19 @@
         <v>200</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>768</v>
+        <v>743</v>
       </c>
       <c r="L65" s="20" t="s">
-        <v>619</v>
+        <v>594</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>620</v>
+        <v>595</v>
       </c>
       <c r="N65" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="O65" s="20" t="s">
         <v>719</v>
-      </c>
-      <c r="O65" s="20" t="s">
-        <v>744</v>
       </c>
       <c r="P65" s="11" t="s">
         <v>201</v>
@@ -5860,13 +5801,13 @@
         <v>30</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>382</v>
+        <v>770</v>
       </c>
       <c r="G66" s="11" t="s">
         <v>32</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>791</v>
+        <v>763</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>21</v>
@@ -5875,17 +5816,17 @@
         <v>146</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>769</v>
+        <v>744</v>
       </c>
       <c r="L66" s="20" t="s">
-        <v>621</v>
+        <v>596</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>622</v>
+        <v>597</v>
       </c>
       <c r="N66" s="11"/>
       <c r="O66" s="20" t="s">
-        <v>709</v>
+        <v>684</v>
       </c>
       <c r="P66" s="11" t="s">
         <v>203</v>
@@ -5908,7 +5849,7 @@
         <v>25</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>382</v>
+        <v>770</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>197</v>
@@ -5923,15 +5864,15 @@
         <v>24</v>
       </c>
       <c r="K67" s="11" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
       <c r="L67" s="20" t="s">
-        <v>623</v>
+        <v>598</v>
       </c>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="20" t="s">
-        <v>624</v>
+        <v>599</v>
       </c>
       <c r="P67" s="11" t="s">
         <v>205</v>
@@ -5954,7 +5895,7 @@
         <v>10</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>459</v>
+        <v>771</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>206</v>
@@ -5969,15 +5910,15 @@
         <v>318</v>
       </c>
       <c r="K68" s="11" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="L68" s="20" t="s">
-        <v>625</v>
+        <v>600</v>
       </c>
       <c r="M68" s="11"/>
       <c r="N68" s="11"/>
       <c r="O68" s="20" t="s">
-        <v>745</v>
+        <v>720</v>
       </c>
       <c r="P68" s="11" t="s">
         <v>207</v>
@@ -6000,7 +5941,7 @@
         <v>15</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>386</v>
+        <v>766</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>197</v>
@@ -6015,15 +5956,15 @@
         <v>16</v>
       </c>
       <c r="K69" s="11" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
       <c r="L69" s="20" t="s">
-        <v>626</v>
+        <v>601</v>
       </c>
       <c r="M69" s="11"/>
       <c r="N69" s="11"/>
       <c r="O69" s="20" t="s">
-        <v>746</v>
+        <v>721</v>
       </c>
       <c r="P69" s="11" t="s">
         <v>209</v>
@@ -6052,24 +5993,24 @@
         <v>32</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>211</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="K70" s="11" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="L70" s="20" t="s">
-        <v>627</v>
+        <v>602</v>
       </c>
       <c r="M70" s="11"/>
       <c r="N70" s="11"/>
       <c r="O70" s="20" t="s">
-        <v>628</v>
+        <v>603</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>212</v>
@@ -6104,18 +6045,18 @@
         <v>21</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="K71" s="11" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="L71" s="20" t="s">
-        <v>629</v>
+        <v>604</v>
       </c>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11" t="s">
-        <v>747</v>
+        <v>722</v>
       </c>
       <c r="P71" s="11" t="s">
         <v>214</v>
@@ -6150,18 +6091,18 @@
         <v>21</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="K72" s="11" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="L72" s="20" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
       <c r="O72" s="20" t="s">
-        <v>748</v>
+        <v>723</v>
       </c>
       <c r="P72" s="11" t="s">
         <v>216</v>
@@ -6187,7 +6128,7 @@
         <v>218</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>241</v>
@@ -6199,16 +6140,16 @@
         <v>24</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
       <c r="L73" s="17" t="s">
-        <v>631</v>
+        <v>606</v>
       </c>
       <c r="M73" s="17" t="s">
-        <v>632</v>
+        <v>607</v>
       </c>
       <c r="O73" s="17" t="s">
-        <v>749</v>
+        <v>724</v>
       </c>
       <c r="P73" s="9" t="s">
         <v>219</v>
@@ -6234,7 +6175,7 @@
         <v>218</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>141</v>
@@ -6243,16 +6184,16 @@
         <v>21</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>633</v>
+        <v>608</v>
       </c>
       <c r="O74" s="8" t="s">
-        <v>750</v>
+        <v>725</v>
       </c>
       <c r="P74" s="9" t="s">
         <v>221</v>
@@ -6278,7 +6219,7 @@
         <v>218</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>90</v>
@@ -6287,16 +6228,16 @@
         <v>211</v>
       </c>
       <c r="J75" s="8" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="L75" s="17" t="s">
-        <v>634</v>
+        <v>609</v>
       </c>
       <c r="O75" s="8" t="s">
-        <v>751</v>
+        <v>726</v>
       </c>
       <c r="P75" s="9" t="s">
         <v>223</v>
@@ -6322,7 +6263,7 @@
         <v>218</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>312</v>
@@ -6331,22 +6272,22 @@
         <v>44</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
       <c r="L76" s="17" t="s">
-        <v>635</v>
+        <v>610</v>
       </c>
       <c r="M76" s="17" t="s">
-        <v>636</v>
+        <v>611</v>
       </c>
       <c r="N76" s="8" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="O76" s="8" t="s">
-        <v>710</v>
+        <v>685</v>
       </c>
       <c r="P76" s="9" t="s">
         <v>225</v>
@@ -6372,7 +6313,7 @@
         <v>218</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>227</v>
@@ -6381,19 +6322,19 @@
         <v>44</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="L77" s="17" t="s">
-        <v>638</v>
+        <v>613</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>639</v>
+        <v>614</v>
       </c>
       <c r="O77" s="8" t="s">
-        <v>752</v>
+        <v>727</v>
       </c>
       <c r="P77" s="9" t="s">
         <v>228</v>
@@ -6419,7 +6360,7 @@
         <v>218</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>227</v>
@@ -6428,19 +6369,19 @@
         <v>44</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
       <c r="L78" s="17" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>714</v>
+        <v>689</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>753</v>
+        <v>728</v>
       </c>
       <c r="P78" s="9" t="s">
         <v>230</v>
@@ -6466,7 +6407,7 @@
         <v>218</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H79" s="8" t="s">
         <v>90</v>
@@ -6478,16 +6419,16 @@
         <v>200</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>466</v>
+        <v>441</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
       <c r="M79" s="8" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="O79" s="17" t="s">
-        <v>754</v>
+        <v>729</v>
       </c>
       <c r="P79" s="9" t="s">
         <v>232</v>
@@ -6513,7 +6454,7 @@
         <v>218</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>90</v>
@@ -6525,16 +6466,16 @@
         <v>200</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="L80" s="17" t="s">
-        <v>643</v>
+        <v>618</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>644</v>
+        <v>619</v>
       </c>
       <c r="O80" s="8" t="s">
-        <v>755</v>
+        <v>730</v>
       </c>
       <c r="P80" s="9" t="s">
         <v>234</v>
@@ -6560,7 +6501,7 @@
         <v>218</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>481</v>
+        <v>456</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>241</v>
@@ -6572,16 +6513,16 @@
         <v>236</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="L81" s="17" t="s">
-        <v>645</v>
+        <v>620</v>
       </c>
       <c r="M81" s="17" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="O81" s="10" t="s">
-        <v>756</v>
+        <v>731</v>
       </c>
       <c r="P81" s="9" t="s">
         <v>237</v>
@@ -6613,25 +6554,25 @@
         <v>241</v>
       </c>
       <c r="I82" s="15" t="s">
-        <v>483</v>
+        <v>458</v>
       </c>
       <c r="J82" s="15" t="s">
         <v>242</v>
       </c>
       <c r="K82" s="17" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>243</v>
       </c>
       <c r="M82" s="17" t="s">
-        <v>647</v>
+        <v>622</v>
       </c>
       <c r="N82" s="17" t="s">
-        <v>648</v>
+        <v>623</v>
       </c>
       <c r="O82" s="17" t="s">
-        <v>649</v>
+        <v>624</v>
       </c>
       <c r="P82" s="15" t="s">
         <v>244</v>
@@ -6660,28 +6601,28 @@
         <v>240</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>484</v>
+        <v>459</v>
       </c>
       <c r="I83" s="15" t="s">
-        <v>485</v>
+        <v>460</v>
       </c>
       <c r="J83" s="15" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="K83" s="17" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="L83" s="17" t="s">
-        <v>650</v>
+        <v>625</v>
       </c>
       <c r="M83" s="17" t="s">
-        <v>651</v>
+        <v>626</v>
       </c>
       <c r="N83" s="17" t="s">
-        <v>652</v>
+        <v>627</v>
       </c>
       <c r="O83" s="17" t="s">
-        <v>715</v>
+        <v>690</v>
       </c>
       <c r="P83" s="15" t="s">
         <v>246</v>
@@ -6719,16 +6660,16 @@
         <v>249</v>
       </c>
       <c r="K84" s="17" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>250</v>
       </c>
       <c r="M84" s="17" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
       <c r="O84" s="17" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
       <c r="P84" s="15" t="s">
         <v>251</v>
@@ -6766,19 +6707,19 @@
         <v>254</v>
       </c>
       <c r="K85" s="17" t="s">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="L85" s="17" t="s">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="M85" s="17" t="s">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="N85" s="17" t="s">
         <v>316</v>
       </c>
       <c r="O85" s="17" t="s">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="P85" s="15" t="s">
         <v>255</v>
@@ -6813,22 +6754,22 @@
         <v>253</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="K86" s="17" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="L86" s="17" t="s">
-        <v>658</v>
+        <v>633</v>
       </c>
       <c r="M86" s="17" t="s">
-        <v>659</v>
+        <v>634</v>
       </c>
       <c r="N86" s="17" t="s">
-        <v>660</v>
+        <v>635</v>
       </c>
       <c r="O86" s="17" t="s">
-        <v>661</v>
+        <v>636</v>
       </c>
       <c r="P86" s="15" t="s">
         <v>257</v>
@@ -6857,28 +6798,28 @@
         <v>74</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>488</v>
+        <v>463</v>
       </c>
       <c r="I87" s="15" t="s">
-        <v>485</v>
+        <v>460</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>127</v>
       </c>
       <c r="K87" s="17" t="s">
-        <v>480</v>
+        <v>455</v>
       </c>
       <c r="L87" s="17" t="s">
-        <v>662</v>
+        <v>637</v>
       </c>
       <c r="M87" s="17" t="s">
-        <v>663</v>
+        <v>638</v>
       </c>
       <c r="N87" s="17" t="s">
-        <v>664</v>
+        <v>639</v>
       </c>
       <c r="O87" s="17" t="s">
-        <v>665</v>
+        <v>640</v>
       </c>
       <c r="P87" s="15" t="s">
         <v>259</v>
@@ -6907,28 +6848,28 @@
         <v>74</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>489</v>
+        <v>464</v>
       </c>
       <c r="I88" s="15" t="s">
-        <v>490</v>
+        <v>465</v>
       </c>
       <c r="J88" s="15" t="s">
         <v>127</v>
       </c>
       <c r="K88" s="17" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
       <c r="L88" s="17" t="s">
-        <v>711</v>
+        <v>686</v>
       </c>
       <c r="M88" s="17" t="s">
-        <v>666</v>
+        <v>641</v>
       </c>
       <c r="N88" s="17" t="s">
-        <v>667</v>
+        <v>642</v>
       </c>
       <c r="O88" s="17" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="P88" s="15" t="s">
         <v>261</v>
@@ -6966,19 +6907,19 @@
         <v>265</v>
       </c>
       <c r="K89" s="17" t="s">
-        <v>770</v>
+        <v>745</v>
       </c>
       <c r="L89" s="17" t="s">
-        <v>669</v>
+        <v>644</v>
       </c>
       <c r="M89" s="17" t="s">
-        <v>670</v>
+        <v>645</v>
       </c>
       <c r="N89" s="17" t="s">
-        <v>671</v>
+        <v>646</v>
       </c>
       <c r="O89" s="17" t="s">
-        <v>672</v>
+        <v>647</v>
       </c>
       <c r="P89" s="15" t="s">
         <v>266</v>
@@ -7016,16 +6957,16 @@
         <v>242</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>771</v>
+        <v>746</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>313</v>
       </c>
       <c r="M90" s="17" t="s">
-        <v>673</v>
+        <v>648</v>
       </c>
       <c r="O90" s="17" t="s">
-        <v>674</v>
+        <v>649</v>
       </c>
       <c r="P90" s="15" t="s">
         <v>269</v>
@@ -7054,7 +6995,7 @@
         <v>74</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>491</v>
+        <v>466</v>
       </c>
       <c r="I91" s="15" t="s">
         <v>264</v>
@@ -7063,16 +7004,16 @@
         <v>271</v>
       </c>
       <c r="K91" s="17" t="s">
-        <v>772</v>
+        <v>747</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>314</v>
       </c>
       <c r="M91" s="17" t="s">
-        <v>675</v>
+        <v>650</v>
       </c>
       <c r="O91" s="17" t="s">
-        <v>720</v>
+        <v>695</v>
       </c>
       <c r="P91" s="15" t="s">
         <v>272</v>
@@ -7101,7 +7042,7 @@
         <v>74</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>484</v>
+        <v>459</v>
       </c>
       <c r="I92" s="15" t="s">
         <v>268</v>
@@ -7110,19 +7051,19 @@
         <v>271</v>
       </c>
       <c r="K92" s="17" t="s">
-        <v>773</v>
+        <v>748</v>
       </c>
       <c r="L92" s="17" t="s">
-        <v>716</v>
+        <v>691</v>
       </c>
       <c r="M92" s="15" t="s">
         <v>274</v>
       </c>
       <c r="N92" s="17" t="s">
-        <v>676</v>
+        <v>651</v>
       </c>
       <c r="O92" s="17" t="s">
-        <v>757</v>
+        <v>732</v>
       </c>
       <c r="P92" s="15" t="s">
         <v>275</v>
@@ -7151,7 +7092,7 @@
         <v>74</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="I93" s="15" t="s">
         <v>264</v>
@@ -7160,19 +7101,19 @@
         <v>277</v>
       </c>
       <c r="K93" s="17" t="s">
-        <v>774</v>
+        <v>749</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>278</v>
       </c>
       <c r="M93" s="17" t="s">
-        <v>677</v>
+        <v>652</v>
       </c>
       <c r="N93" s="17" t="s">
-        <v>678</v>
+        <v>653</v>
       </c>
       <c r="O93" s="17" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="P93" s="15" t="s">
         <v>279</v>
@@ -7201,28 +7142,28 @@
         <v>74</v>
       </c>
       <c r="H94" s="15" t="s">
-        <v>493</v>
+        <v>468</v>
       </c>
       <c r="I94" s="15" t="s">
-        <v>494</v>
+        <v>469</v>
       </c>
       <c r="J94" s="15" t="s">
-        <v>495</v>
+        <v>470</v>
       </c>
       <c r="K94" s="17" t="s">
-        <v>775</v>
+        <v>750</v>
       </c>
       <c r="L94" s="17" t="s">
-        <v>679</v>
+        <v>654</v>
       </c>
       <c r="M94" s="17" t="s">
-        <v>680</v>
+        <v>655</v>
       </c>
       <c r="N94" s="17" t="s">
-        <v>681</v>
+        <v>656</v>
       </c>
       <c r="O94" s="17" t="s">
-        <v>682</v>
+        <v>657</v>
       </c>
       <c r="P94" s="15" t="s">
         <v>281</v>
@@ -7257,22 +7198,22 @@
         <v>283</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>496</v>
+        <v>471</v>
       </c>
       <c r="K95" s="17" t="s">
-        <v>776</v>
+        <v>751</v>
       </c>
       <c r="L95" s="17" t="s">
-        <v>683</v>
+        <v>658</v>
       </c>
       <c r="M95" s="17" t="s">
-        <v>684</v>
+        <v>659</v>
       </c>
       <c r="N95" s="17" t="s">
-        <v>685</v>
+        <v>660</v>
       </c>
       <c r="O95" s="17" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
       <c r="P95" s="15" t="s">
         <v>284</v>
@@ -7310,16 +7251,16 @@
         <v>242</v>
       </c>
       <c r="K96" s="17" t="s">
-        <v>777</v>
+        <v>752</v>
       </c>
       <c r="L96" s="17" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
       <c r="M96" s="17" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
       <c r="O96" s="17" t="s">
-        <v>717</v>
+        <v>692</v>
       </c>
       <c r="P96" s="15" t="s">
         <v>286</v>
@@ -7357,19 +7298,19 @@
         <v>242</v>
       </c>
       <c r="K97" s="17" t="s">
-        <v>778</v>
+        <v>753</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>290</v>
       </c>
       <c r="M97" s="17" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
       <c r="N97" s="17" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
       <c r="O97" s="17" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
       <c r="P97" s="15" t="s">
         <v>291</v>
@@ -7398,28 +7339,28 @@
         <v>293</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
       <c r="I98" s="15" t="s">
-        <v>498</v>
+        <v>473</v>
       </c>
       <c r="J98" s="15" t="s">
         <v>294</v>
       </c>
       <c r="K98" s="17" t="s">
-        <v>779</v>
+        <v>754</v>
       </c>
       <c r="L98" s="15" t="s">
         <v>295</v>
       </c>
       <c r="M98" s="17" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
       <c r="N98" s="17" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
       <c r="O98" s="17" t="s">
-        <v>694</v>
+        <v>669</v>
       </c>
       <c r="P98" s="15" t="s">
         <v>296</v>
@@ -7448,28 +7389,28 @@
         <v>74</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>499</v>
+        <v>474</v>
       </c>
       <c r="I99" s="15" t="s">
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="J99" s="15" t="s">
-        <v>501</v>
+        <v>476</v>
       </c>
       <c r="K99" s="17" t="s">
-        <v>780</v>
+        <v>755</v>
       </c>
       <c r="L99" s="17" t="s">
-        <v>695</v>
+        <v>670</v>
       </c>
       <c r="M99" s="17" t="s">
-        <v>696</v>
+        <v>671</v>
       </c>
       <c r="N99" s="17" t="s">
-        <v>697</v>
+        <v>672</v>
       </c>
       <c r="O99" s="17" t="s">
-        <v>698</v>
+        <v>673</v>
       </c>
       <c r="P99" s="15" t="s">
         <v>298</v>
@@ -7498,28 +7439,28 @@
         <v>293</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
       <c r="I100" s="15" t="s">
-        <v>498</v>
+        <v>473</v>
       </c>
       <c r="J100" s="15" t="s">
         <v>300</v>
       </c>
       <c r="K100" s="17" t="s">
-        <v>781</v>
+        <v>756</v>
       </c>
       <c r="L100" s="17" t="s">
-        <v>699</v>
+        <v>674</v>
       </c>
       <c r="M100" s="17" t="s">
-        <v>700</v>
+        <v>675</v>
       </c>
       <c r="N100" s="17" t="s">
-        <v>701</v>
+        <v>676</v>
       </c>
       <c r="O100" s="17" t="s">
-        <v>702</v>
+        <v>677</v>
       </c>
       <c r="P100" s="15" t="s">
         <v>301</v>
@@ -7557,16 +7498,16 @@
         <v>305</v>
       </c>
       <c r="K101" s="17" t="s">
-        <v>782</v>
+        <v>757</v>
       </c>
       <c r="L101" s="15" t="s">
         <v>315</v>
       </c>
       <c r="M101" s="17" t="s">
-        <v>703</v>
+        <v>678</v>
       </c>
       <c r="O101" s="17" t="s">
-        <v>704</v>
+        <v>679</v>
       </c>
       <c r="P101" s="15" t="s">
         <v>306</v>
@@ -7633,6 +7574,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008391A78A96E52D49B7547661E7A4BF06" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f85b5808450112fb8a7ca44957bb917">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40cda520-8ac8-43fb-9853-1ab640917454" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4771e6a9242bec3fb156c39d4a4cbe5" ns2:_="">
     <xsd:import namespace="40cda520-8ac8-43fb-9853-1ab640917454"/>
@@ -7780,35 +7736,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF8687-F08D-4160-94B0-189397DE676C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FC7F45C-4F37-4DFF-BDAF-78C0D0B5C911}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40cda520-8ac8-43fb-9853-1ab640917454"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7830,9 +7761,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FC7F45C-4F37-4DFF-BDAF-78C0D0B5C911}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF8687-F08D-4160-94B0-189397DE676C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40cda520-8ac8-43fb-9853-1ab640917454"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>